<commit_message>
Updated the spreadsheet on github
</commit_message>
<xml_diff>
--- a/proto/wage-subsidy/calculator.xlsx
+++ b/proto/wage-subsidy/calculator.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crf000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mborgesp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <definedName name="claimPeriods">'Claim periods'!$A$1:$A$4</definedName>
     <definedName name="otherEmployees">'Per week calculation'!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>Week 1</t>
   </si>
@@ -132,36 +132,7 @@
     <t>Canada.ca Wage subsidy calculator (canada.ca/calculate-wage-subsidy)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">An </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>arm's length employee</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is connected by blood relationship, marriage or common-law partnership or adoption. Blood relationships do not normally include aunts, uncles, nieces, nephews, or cousins for purposes of the Income Tax Act.</t>
-    </r>
-  </si>
-  <si>
     <t>Go to the other tab "Per week calculation" -&gt;</t>
-  </si>
-  <si>
-    <t>Once you've finished inputting all employee earning amounts in the other tab, use the "Value to use in step 2" at the beginning of this sheet to finish your calculation on Canada.ca</t>
   </si>
   <si>
     <t>Employee name</t>
@@ -181,31 +152,6 @@
   </si>
   <si>
     <t>*3</t>
-  </si>
-  <si>
-    <r>
-      <t>For every employee not reflected in 2a or 2b (employees that earn less than $1,130 CND or who are non-arm's length*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>), in the sheet "Per week calculation", you will have to input their</t>
-    </r>
   </si>
   <si>
     <r>
@@ -266,6 +212,61 @@
     <t>Notes:</t>
   </si>
   <si>
+    <t>Employee amount (calculated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Weekly gross earnings for each week of the period selected in step 1.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Arm's length:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Generally, an arm's-length employee includes any employee who does not own the business (or in the case of a corporation, control the corporation) and is not a member of that person's immediate family.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Non-arm's length (not at arm's length): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A non-arm's-length employee is someone who owns the business (or In the case of a corporation, controls the corporation) or is part of that person's immediate family.</t>
+    </r>
+  </si>
+  <si>
+    <t>For every employee not reflected in 2a or 2b (employees who are non-arm's length*1 or employees that have had a decrease in pay), in the sheet "Per week calculation", you will have to input their</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Any period of over 7 consecutive days during which no pay was received </t>
     </r>
@@ -288,27 +289,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, such as for leave from work can be ommitted from the average baseline pay.</t>
+      <t>, such as for leave from work can be omitted from the average baseline pay.</t>
     </r>
   </si>
   <si>
-    <t>The total base CEWS calculated in this spreadsheet does not include deductions. Complete continue from step 3 on Canada.ca for the actual CEWS amount.</t>
+    <t>The total base CEWS calculated in this spreadsheet does not include deductions. Continue from step 3 on Canada.ca for the actual CEWS amount.</t>
   </si>
   <si>
-    <t>Employee amount (calculated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Weekly gross earnings for each week of the period selected in step 1.</t>
+    <t>Once you've completed all employee earning amounts in the Per week calculation tab, use the amount in "Value to use in step 2" at the beginning of this sheet to finish your calculation on Canada.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,13 +412,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -719,16 +710,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -744,7 +735,7 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -776,10 +767,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -789,22 +780,16 @@
     <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -814,10 +799,10 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -831,6 +816,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,9 +1121,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="89" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
       <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
@@ -1155,24 +1146,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="6"/>
@@ -1247,8 +1238,8 @@
       <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="63" t="s">
-        <v>37</v>
+      <c r="B6" s="61" t="s">
+        <v>35</v>
       </c>
       <c r="C6" s="7"/>
       <c r="F6" s="6"/>
@@ -1264,21 +1255,21 @@
       <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="64"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="65" t="str">
+      <c r="D7" s="63" t="str">
         <f>"Total base CEWS "&amp;Instructions!C14</f>
         <v>Total base CEWS Select a claim period</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="65" t="str">
+      <c r="H7" s="63" t="str">
         <f>"Total gross payroll "&amp;Instructions!C14</f>
         <v>Total gross payroll Select a claim period</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="65" t="str">
+      <c r="L7" s="63" t="str">
         <f>"Total number of employees "&amp;Instructions!C14</f>
         <v>Total number of employees Select a claim period</v>
       </c>
@@ -1289,15 +1280,15 @@
     <row r="8" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="34"/>
       <c r="C8" s="44"/>
-      <c r="D8" s="66"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="45"/>
       <c r="F8" s="6"/>
       <c r="G8" s="44"/>
-      <c r="H8" s="66"/>
+      <c r="H8" s="64"/>
       <c r="I8" s="45"/>
       <c r="J8" s="6"/>
       <c r="K8" s="44"/>
-      <c r="L8" s="66"/>
+      <c r="L8" s="64"/>
       <c r="M8" s="45"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -1394,11 +1385,11 @@
       <c r="B14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
@@ -1410,19 +1401,19 @@
       <c r="A16" s="23">
         <v>2</v>
       </c>
-      <c r="B16" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
+      <c r="B16" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -1440,7 +1431,7 @@
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -1465,7 +1456,7 @@
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="6"/>
@@ -1479,7 +1470,7 @@
     <row r="21" spans="1:16" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="11"/>
@@ -1494,63 +1485,64 @@
     <row r="22" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
+        <v>37</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
     </row>
     <row r="23" spans="1:16" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="13"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-    </row>
-    <row r="24" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="70"/>
+    </row>
+    <row r="24" spans="1:16" s="7" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
-      <c r="B24" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="51" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-    </row>
-    <row r="25" spans="1:16" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="70"/>
+      <c r="N24" s="70"/>
+    </row>
+    <row r="25" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
@@ -1563,8 +1555,12 @@
     </row>
     <row r="26" spans="1:16" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="51"/>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>50</v>
+      </c>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
@@ -1574,47 +1570,54 @@
       <c r="J26" s="51"/>
       <c r="K26" s="51"/>
     </row>
-    <row r="27" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+    <row r="27" spans="1:16" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+    </row>
+    <row r="28" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
         <v>3</v>
       </c>
-      <c r="B27" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-    </row>
-    <row r="28" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
     </row>
     <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="31" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+    <row r="30" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="32" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="K32" s="6"/>
@@ -1623,12 +1626,12 @@
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B34" s="3"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
@@ -1640,24 +1643,31 @@
       <c r="N35" s="6"/>
     </row>
     <row r="36" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="B36" s="3"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
+    <row r="37" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="C22:N23"/>
-    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="C24:N24"/>
+    <mergeCell ref="B28:L28"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="H7:H8"/>
@@ -1672,7 +1682,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="2b" display="Step 2b in the Wage subsidy calculation on Canada.ca"/>
-    <hyperlink ref="C28" r:id="rId2" location="2b" display="Step 2b in the Wage subsidy calculation on Canada.ca"/>
+    <hyperlink ref="C29" r:id="rId2" location="2b" display="Step 2b in the Wage subsidy calculation on Canada.ca"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1709,7 +1719,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="18"/>
       <c r="H1" s="73" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I1" s="73"/>
       <c r="J1" s="73"/>
@@ -1718,10 +1728,10 @@
     </row>
     <row r="2" spans="1:12" s="48" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>0</v>
@@ -1736,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H2" s="52" t="s">
         <v>0</v>
@@ -1751,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="53" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="49" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -57088,7 +57098,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="An arm's length employee is connected by blood relationship, marriage or common-law partnership or adoption. Blood relationships do not normally include aunts, uncles, nieces, nephews, or cousins for purposes of the Income Tax Act." sqref="G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Arm's length: Generally, an arm's-length employee includes any employee who does not own the business (or in the case of a corporation, control the corporation) and is not a member of that person's immediate family." sqref="G2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any period of over 7 consecutive days during which no pay was received such as for leave from work can be ommitted from the average." sqref="B2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The total base CEWS calculated in this spreadsheet does not include deductions. Complete continue from step 3 on Canada.ca for the actual CEWS amount." sqref="L2"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1048576">
@@ -57186,7 +57196,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -57230,7 +57240,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -57274,7 +57284,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -57318,7 +57328,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>